<commit_message>
Update results after SwingLow bug fix
Results regenerated with corrected directional bar detection.
All tests pass with 100% accuracy on Gann data.

Best signal per stock summary:
- Reversal: best for 13 stocks (avg 17.3% return, 74.2% win)
- TwelveBar: best for 7 stocks (avg 26.8% return, 76.6% win)
- Bullish: best for 8 stocks (avg 16.9% return, 71.6% win)

Top performers: FMG 87.7%, CSL 28.6%, RMD 28.5%, GMG 26.3%

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/results/SHL.xlsx
+++ b/results/SHL.xlsx
@@ -6949,26 +6949,26 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>240</v>
+        <v>174</v>
       </c>
       <c r="C135" t="inlineStr"/>
       <c r="D135" t="n">
-        <v>0.0350663512945175</v>
+        <v>0.0207210145890712</v>
       </c>
       <c r="E135" t="n">
-        <v>572.7273152214607</v>
+        <v>23.07704339337198</v>
       </c>
       <c r="F135" t="b">
         <v>1</v>
       </c>
       <c r="G135" t="n">
-        <v>572.7273152214607</v>
+        <v>84.61552014425855</v>
       </c>
       <c r="H135" t="n">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="I135" t="n">
-        <v>0</v>
+        <v>-30.76922547887741</v>
       </c>
       <c r="J135" t="n">
         <v>0</v>
@@ -6979,7 +6979,7 @@
       <c r="L135" t="inlineStr"/>
       <c r="M135" t="inlineStr"/>
       <c r="N135" t="n">
-        <v>0</v>
+        <v>61.53847675088657</v>
       </c>
       <c r="O135" t="inlineStr"/>
       <c r="P135" t="inlineStr"/>
@@ -9054,22 +9054,22 @@
         <v>62.5</v>
       </c>
       <c r="D4" t="n">
-        <v>25.02995961310444</v>
+        <v>11.28870281740222</v>
       </c>
       <c r="E4" t="n">
         <v>9.227112236985972</v>
       </c>
       <c r="F4" t="n">
-        <v>92.77179022352327</v>
+        <v>26.85962196794551</v>
       </c>
       <c r="G4" t="n">
-        <v>39.4362653708699</v>
+        <v>27.23347049393985</v>
       </c>
       <c r="H4" t="n">
-        <v>-14.88676692872951</v>
+        <v>-15.65599756570144</v>
       </c>
       <c r="I4" t="n">
-        <v>14.40630575776546</v>
+        <v>15.94476767653763</v>
       </c>
       <c r="J4" t="n">
         <v>75</v>

</xml_diff>